<commit_message>
implements threshold logic for context scores
</commit_message>
<xml_diff>
--- a/inst/extdata/Contextual Computation V0.3 - Live Version.xlsx
+++ b/inst/extdata/Contextual Computation V0.3 - Live Version.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg.sharepoint.com/sites/EIOSCoreTeamIII/Shared Documents/Data Science for PHI/SPA-data-science/SPA-algorithm-demo/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg.sharepoint.com/sites/EIOSCoreTeamIII/Shared Documents/Data Science for PHI/SPA-data-science/SPA.Algorithm.Demo/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="752" documentId="8_{10126B69-836C-4F71-8DB2-60A07635146C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0B10FC4-58FE-46BD-A717-850C1F9FE02B}"/>
   <bookViews>
-    <workbookView xWindow="2805" yWindow="2805" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{DFFCEFC9-B090-4D4D-8D52-53EBE2FF3297}"/>
+    <workbookView xWindow="2800" yWindow="2800" windowWidth="21600" windowHeight="11380" xr2:uid="{DFFCEFC9-B090-4D4D-8D52-53EBE2FF3297}"/>
   </bookViews>
   <sheets>
     <sheet name="Contextual Computation" sheetId="1" r:id="rId1"/>
@@ -1363,21 +1363,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4E8345-E56A-4104-A2CC-5D008640BF5B}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B7"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="23.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="3" customWidth="1"/>
+    <col min="1" max="2" width="23.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="89" style="13" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="3"/>
-    <col min="6" max="6" width="42.42578125" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="5" max="5" width="9.1640625" style="3"/>
+    <col min="6" max="6" width="42.5" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
         <v>4</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="28"/>
       <c r="B3" s="29"/>
       <c r="C3" s="28"/>
@@ -1413,7 +1413,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="99" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
         <v>9</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="30"/>
       <c r="B5" s="29"/>
       <c r="C5" s="28"/>
@@ -1435,7 +1435,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="104.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
         <v>14</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="28"/>
       <c r="B7" s="29"/>
       <c r="C7" s="28"/>
@@ -1457,7 +1457,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="198.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="198.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -1472,7 +1472,7 @@
       </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="111.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>22</v>
       </c>
@@ -1507,6 +1507,7 @@
     <hyperlink ref="B8" r:id="rId5" xr:uid="{4F3D7DB9-32F1-4CB9-B481-03732638AAB2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1514,21 +1515,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0787B019-9136-4FBD-8545-DF14C53F3423}">
   <dimension ref="A1:G193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="26.5" customWidth="1"/>
+    <col min="8" max="8" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>25</v>
       </c>
@@ -1545,7 +1546,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>30</v>
       </c>
@@ -1562,7 +1563,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>33</v>
       </c>
@@ -1579,7 +1580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>34</v>
       </c>
@@ -1596,7 +1597,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>35</v>
       </c>
@@ -1613,7 +1614,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>36</v>
       </c>
@@ -1630,7 +1631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>37</v>
       </c>
@@ -1641,7 +1642,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>38</v>
       </c>
@@ -1652,7 +1653,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>39</v>
       </c>
@@ -1666,7 +1667,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>40</v>
       </c>
@@ -1683,7 +1684,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>41</v>
       </c>
@@ -1694,7 +1695,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>42</v>
       </c>
@@ -1711,7 +1712,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>43</v>
       </c>
@@ -1722,7 +1723,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>44</v>
       </c>
@@ -1739,7 +1740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>45</v>
       </c>
@@ -1756,7 +1757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>46</v>
       </c>
@@ -1767,7 +1768,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>47</v>
       </c>
@@ -1778,7 +1779,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>48</v>
       </c>
@@ -1795,7 +1796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>49</v>
       </c>
@@ -1806,7 +1807,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>50</v>
       </c>
@@ -1817,7 +1818,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>51</v>
       </c>
@@ -1834,7 +1835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>52</v>
       </c>
@@ -1845,7 +1846,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>53</v>
       </c>
@@ -1856,7 +1857,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>54</v>
       </c>
@@ -1873,7 +1874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>55</v>
       </c>
@@ -1884,7 +1885,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>56</v>
       </c>
@@ -1901,7 +1902,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
         <v>57</v>
       </c>
@@ -1912,7 +1913,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>58</v>
       </c>
@@ -1929,7 +1930,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>59</v>
       </c>
@@ -1946,7 +1947,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>60</v>
       </c>
@@ -1963,7 +1964,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
         <v>61</v>
       </c>
@@ -1980,7 +1981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
         <v>62</v>
       </c>
@@ -1997,7 +1998,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>63</v>
       </c>
@@ -2014,7 +2015,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
         <v>64</v>
       </c>
@@ -2025,7 +2026,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
         <v>65</v>
       </c>
@@ -2042,7 +2043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
         <v>66</v>
       </c>
@@ -2053,7 +2054,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
         <v>67</v>
       </c>
@@ -2064,7 +2065,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>68</v>
       </c>
@@ -2075,7 +2076,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
         <v>69</v>
       </c>
@@ -2092,7 +2093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
         <v>70</v>
       </c>
@@ -2109,7 +2110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
         <v>71</v>
       </c>
@@ -2126,7 +2127,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
         <v>72</v>
       </c>
@@ -2137,7 +2138,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
         <v>73</v>
       </c>
@@ -2154,7 +2155,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
         <v>74</v>
       </c>
@@ -2165,7 +2166,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
         <v>75</v>
       </c>
@@ -2176,7 +2177,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
         <v>76</v>
       </c>
@@ -2187,7 +2188,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
         <v>77</v>
       </c>
@@ -2198,7 +2199,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
         <v>78</v>
       </c>
@@ -2209,7 +2210,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
         <v>79</v>
       </c>
@@ -2226,7 +2227,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
         <v>80</v>
       </c>
@@ -2237,7 +2238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="17" t="s">
         <v>81</v>
       </c>
@@ -2248,7 +2249,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="17" t="s">
         <v>82</v>
       </c>
@@ -2259,7 +2260,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
         <v>83</v>
       </c>
@@ -2270,7 +2271,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="17" t="s">
         <v>84</v>
       </c>
@@ -2281,7 +2282,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="17" t="s">
         <v>85</v>
       </c>
@@ -2292,7 +2293,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="17" t="s">
         <v>86</v>
       </c>
@@ -2309,7 +2310,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="17" t="s">
         <v>87</v>
       </c>
@@ -2320,7 +2321,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="17" t="s">
         <v>88</v>
       </c>
@@ -2337,7 +2338,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="17" t="s">
         <v>89</v>
       </c>
@@ -2354,7 +2355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="17" t="s">
         <v>90</v>
       </c>
@@ -2365,7 +2366,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="17" t="s">
         <v>91</v>
       </c>
@@ -2382,7 +2383,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="17" t="s">
         <v>92</v>
       </c>
@@ -2393,7 +2394,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="17" t="s">
         <v>93</v>
       </c>
@@ -2404,7 +2405,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="17" t="s">
         <v>94</v>
       </c>
@@ -2421,7 +2422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="17" t="s">
         <v>95</v>
       </c>
@@ -2438,7 +2439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="17" t="s">
         <v>96</v>
       </c>
@@ -2449,7 +2450,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="17" t="s">
         <v>97</v>
       </c>
@@ -2466,7 +2467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="17" t="s">
         <v>98</v>
       </c>
@@ -2477,7 +2478,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="17" t="s">
         <v>99</v>
       </c>
@@ -2488,7 +2489,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="17" t="s">
         <v>100</v>
       </c>
@@ -2499,7 +2500,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="17" t="s">
         <v>101</v>
       </c>
@@ -2516,7 +2517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="17" t="s">
         <v>102</v>
       </c>
@@ -2533,7 +2534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="17" t="s">
         <v>103</v>
       </c>
@@ -2544,7 +2545,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="17" t="s">
         <v>104</v>
       </c>
@@ -2555,7 +2556,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="17" t="s">
         <v>105</v>
       </c>
@@ -2566,7 +2567,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="17" t="s">
         <v>106</v>
       </c>
@@ -2577,7 +2578,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="17" t="s">
         <v>107</v>
       </c>
@@ -2588,7 +2589,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="17" t="s">
         <v>108</v>
       </c>
@@ -2599,7 +2600,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="17" t="s">
         <v>109</v>
       </c>
@@ -2616,7 +2617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="17" t="s">
         <v>110</v>
       </c>
@@ -2627,7 +2628,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="17" t="s">
         <v>111</v>
       </c>
@@ -2644,7 +2645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="17" t="s">
         <v>112</v>
       </c>
@@ -2655,7 +2656,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="17" t="s">
         <v>113</v>
       </c>
@@ -2666,7 +2667,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="17" t="s">
         <v>114</v>
       </c>
@@ -2677,7 +2678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="17" t="s">
         <v>115</v>
       </c>
@@ -2688,7 +2689,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="17" t="s">
         <v>116</v>
       </c>
@@ -2705,7 +2706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="17" t="s">
         <v>117</v>
       </c>
@@ -2722,7 +2723,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="17" t="s">
         <v>118</v>
       </c>
@@ -2733,7 +2734,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="17" t="s">
         <v>119</v>
       </c>
@@ -2750,7 +2751,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="17" t="s">
         <v>120</v>
       </c>
@@ -2761,7 +2762,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="17" t="s">
         <v>121</v>
       </c>
@@ -2772,7 +2773,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="17" t="s">
         <v>122</v>
       </c>
@@ -2789,7 +2790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="17" t="s">
         <v>123</v>
       </c>
@@ -2806,7 +2807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="17" t="s">
         <v>124</v>
       </c>
@@ -2823,7 +2824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="17" t="s">
         <v>125</v>
       </c>
@@ -2840,7 +2841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="17" t="s">
         <v>126</v>
       </c>
@@ -2857,7 +2858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="17" t="s">
         <v>127</v>
       </c>
@@ -2874,7 +2875,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="17" t="s">
         <v>128</v>
       </c>
@@ -2891,7 +2892,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="17" t="s">
         <v>129</v>
       </c>
@@ -2908,7 +2909,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="17" t="s">
         <v>130</v>
       </c>
@@ -2925,7 +2926,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="17" t="s">
         <v>131</v>
       </c>
@@ -2939,7 +2940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="17" t="s">
         <v>132</v>
       </c>
@@ -2956,7 +2957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="17" t="s">
         <v>133</v>
       </c>
@@ -2967,7 +2968,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="17" t="s">
         <v>134</v>
       </c>
@@ -2984,7 +2985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="17" t="s">
         <v>135</v>
       </c>
@@ -3001,7 +3002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="17" t="s">
         <v>136</v>
       </c>
@@ -3018,7 +3019,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="17" t="s">
         <v>137</v>
       </c>
@@ -3035,7 +3036,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="17" t="s">
         <v>138</v>
       </c>
@@ -3052,7 +3053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="17" t="s">
         <v>139</v>
       </c>
@@ -3063,7 +3064,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="17" t="s">
         <v>140</v>
       </c>
@@ -3080,7 +3081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="17" t="s">
         <v>141</v>
       </c>
@@ -3097,7 +3098,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="17" t="s">
         <v>142</v>
       </c>
@@ -3114,7 +3115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" s="17" t="s">
         <v>143</v>
       </c>
@@ -3125,7 +3126,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" s="17" t="s">
         <v>144</v>
       </c>
@@ -3136,7 +3137,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" s="17" t="s">
         <v>145</v>
       </c>
@@ -3153,7 +3154,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="17" t="s">
         <v>146</v>
       </c>
@@ -3170,7 +3171,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" s="17" t="s">
         <v>147</v>
       </c>
@@ -3187,7 +3188,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="17" t="s">
         <v>148</v>
       </c>
@@ -3204,7 +3205,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="17" t="s">
         <v>149</v>
       </c>
@@ -3221,7 +3222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="17" t="s">
         <v>150</v>
       </c>
@@ -3238,7 +3239,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" s="17" t="s">
         <v>151</v>
       </c>
@@ -3255,7 +3256,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" s="17" t="s">
         <v>152</v>
       </c>
@@ -3266,7 +3267,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" s="17" t="s">
         <v>153</v>
       </c>
@@ -3283,7 +3284,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" s="17" t="s">
         <v>154</v>
       </c>
@@ -3294,7 +3295,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="17" t="s">
         <v>155</v>
       </c>
@@ -3311,7 +3312,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" s="17" t="s">
         <v>156</v>
       </c>
@@ -3322,7 +3323,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" s="17" t="s">
         <v>157</v>
       </c>
@@ -3339,7 +3340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" s="17" t="s">
         <v>158</v>
       </c>
@@ -3356,7 +3357,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" s="17" t="s">
         <v>159</v>
       </c>
@@ -3373,7 +3374,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="17" t="s">
         <v>160</v>
       </c>
@@ -3384,7 +3385,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" s="17" t="s">
         <v>161</v>
       </c>
@@ -3401,7 +3402,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" s="17" t="s">
         <v>162</v>
       </c>
@@ -3418,7 +3419,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" s="17" t="s">
         <v>163</v>
       </c>
@@ -3435,7 +3436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" s="17" t="s">
         <v>164</v>
       </c>
@@ -3446,7 +3447,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" s="17" t="s">
         <v>165</v>
       </c>
@@ -3457,7 +3458,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="17" t="s">
         <v>166</v>
       </c>
@@ -3468,7 +3469,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="17" t="s">
         <v>167</v>
       </c>
@@ -3479,7 +3480,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" s="17" t="s">
         <v>168</v>
       </c>
@@ -3490,7 +3491,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" s="17" t="s">
         <v>169</v>
       </c>
@@ -3507,7 +3508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" s="17" t="s">
         <v>170</v>
       </c>
@@ -3518,7 +3519,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" s="17" t="s">
         <v>171</v>
       </c>
@@ -3529,7 +3530,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" s="17" t="s">
         <v>172</v>
       </c>
@@ -3546,7 +3547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" s="17" t="s">
         <v>173</v>
       </c>
@@ -3557,7 +3558,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" s="17" t="s">
         <v>174</v>
       </c>
@@ -3568,7 +3569,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" s="17" t="s">
         <v>175</v>
       </c>
@@ -3585,7 +3586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" s="17" t="s">
         <v>176</v>
       </c>
@@ -3596,7 +3597,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" s="17" t="s">
         <v>177</v>
       </c>
@@ -3607,7 +3608,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" s="17" t="s">
         <v>178</v>
       </c>
@@ -3618,7 +3619,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" s="17" t="s">
         <v>179</v>
       </c>
@@ -3629,7 +3630,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" s="17" t="s">
         <v>180</v>
       </c>
@@ -3646,7 +3647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" s="17" t="s">
         <v>181</v>
       </c>
@@ -3663,7 +3664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" s="17" t="s">
         <v>182</v>
       </c>
@@ -3680,7 +3681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" s="17" t="s">
         <v>183</v>
       </c>
@@ -3697,7 +3698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" s="17" t="s">
         <v>184</v>
       </c>
@@ -3714,7 +3715,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" s="17" t="s">
         <v>185</v>
       </c>
@@ -3731,7 +3732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" s="17" t="s">
         <v>186</v>
       </c>
@@ -3748,7 +3749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" s="17" t="s">
         <v>187</v>
       </c>
@@ -3759,7 +3760,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" s="17" t="s">
         <v>188</v>
       </c>
@@ -3776,7 +3777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" s="17" t="s">
         <v>189</v>
       </c>
@@ -3790,7 +3791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" s="17" t="s">
         <v>190</v>
       </c>
@@ -3807,7 +3808,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" s="17" t="s">
         <v>191</v>
       </c>
@@ -3824,7 +3825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" s="17" t="s">
         <v>192</v>
       </c>
@@ -3841,7 +3842,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" s="17" t="s">
         <v>193</v>
       </c>
@@ -3852,7 +3853,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" s="17" t="s">
         <v>194</v>
       </c>
@@ -3869,7 +3870,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" s="17" t="s">
         <v>195</v>
       </c>
@@ -3886,7 +3887,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" s="17" t="s">
         <v>196</v>
       </c>
@@ -3897,7 +3898,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" s="17" t="s">
         <v>197</v>
       </c>
@@ -3908,7 +3909,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" s="17" t="s">
         <v>198</v>
       </c>
@@ -3925,7 +3926,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" s="17" t="s">
         <v>199</v>
       </c>
@@ -3942,7 +3943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" s="17" t="s">
         <v>200</v>
       </c>
@@ -3959,7 +3960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" s="17" t="s">
         <v>201</v>
       </c>
@@ -3976,7 +3977,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" s="17" t="s">
         <v>202</v>
       </c>
@@ -3993,7 +3994,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" s="17" t="s">
         <v>203</v>
       </c>
@@ -4007,7 +4008,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" s="17" t="s">
         <v>204</v>
       </c>
@@ -4024,7 +4025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" s="17" t="s">
         <v>205</v>
       </c>
@@ -4038,7 +4039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" s="17" t="s">
         <v>206</v>
       </c>
@@ -4049,7 +4050,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" s="17" t="s">
         <v>207</v>
       </c>
@@ -4066,7 +4067,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" s="17" t="s">
         <v>208</v>
       </c>
@@ -4077,7 +4078,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" s="17" t="s">
         <v>209</v>
       </c>
@@ -4088,7 +4089,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" s="17" t="s">
         <v>210</v>
       </c>
@@ -4099,7 +4100,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" s="17" t="s">
         <v>211</v>
       </c>
@@ -4116,7 +4117,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" s="17" t="s">
         <v>212</v>
       </c>
@@ -4133,7 +4134,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" s="17" t="s">
         <v>213</v>
       </c>
@@ -4150,7 +4151,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" s="17" t="s">
         <v>214</v>
       </c>
@@ -4161,7 +4162,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" s="17" t="s">
         <v>215</v>
       </c>
@@ -4178,7 +4179,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" s="17" t="s">
         <v>216</v>
       </c>
@@ -4189,7 +4190,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" s="17" t="s">
         <v>217</v>
       </c>
@@ -4206,7 +4207,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" s="17" t="s">
         <v>218</v>
       </c>
@@ -4217,7 +4218,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" s="17" t="s">
         <v>219</v>
       </c>
@@ -4228,7 +4229,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" s="17" t="s">
         <v>220</v>
       </c>
@@ -4245,7 +4246,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" s="17" t="s">
         <v>221</v>
       </c>
@@ -4256,7 +4257,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" s="17" t="s">
         <v>222</v>
       </c>
@@ -4270,7 +4271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193" s="17" t="s">
         <v>223</v>
       </c>
@@ -4293,12 +4294,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="97c8a684-1c4b-4244-9323-fa8d251df7dc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="97eadeb2-cd7a-457f-ac14-0ed0556ce061">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Notes xmlns="97eadeb2-cd7a-457f-ac14-0ed0556ce061" xsi:nil="true"/>
+    <Status xmlns="97eadeb2-cd7a-457f-ac14-0ed0556ce061" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4573,22 +4578,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="97c8a684-1c4b-4244-9323-fa8d251df7dc" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="97eadeb2-cd7a-457f-ac14-0ed0556ce061">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Notes xmlns="97eadeb2-cd7a-457f-ac14-0ed0556ce061" xsi:nil="true"/>
-    <Status xmlns="97eadeb2-cd7a-457f-ac14-0ed0556ce061" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C61BAB8-0D87-4815-A441-9E89F437AF00}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5379F056-A4DA-4515-98E0-F3C70C1D5F8D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="97c8a684-1c4b-4244-9323-fa8d251df7dc"/>
+    <ds:schemaRef ds:uri="97eadeb2-cd7a-457f-ac14-0ed0556ce061"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4613,12 +4623,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5379F056-A4DA-4515-98E0-F3C70C1D5F8D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C61BAB8-0D87-4815-A441-9E89F437AF00}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="97c8a684-1c4b-4244-9323-fa8d251df7dc"/>
-    <ds:schemaRef ds:uri="97eadeb2-cd7a-457f-ac14-0ed0556ce061"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>